<commit_message>
Updates to database and added functions
Updates:
- Included "Status" to the table "Product" to avoid partial dependecy. Also changed the data type of status to a boolean. If an object is rented, its status is set to TRUE, not rented is FALSE. Once a product is returned, its status is then reset to FALSE. The Table "Student Inventory" will then remove records where Status == FALSE

- Coded a program to register new users that do not exist in database.

- Changed sql and Excel  file according the previously mentioned changes
</commit_message>
<xml_diff>
--- a/SLS/Database/SLS - Normalisering.xlsx
+++ b/SLS/Database/SLS - Normalisering.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9cc3541a4def9e10/Dokumenter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9cc3541a4def9e10/Dokumenter/USN/DDA/SLS/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{621C04C8-C7F1-48B0-BD19-D8DD9ACFBFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B556D60-B411-4C08-B717-A2BDA4B084BE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{576927ED-C296-421D-BD9A-19916A12A644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="6" xr2:uid="{014C386D-7984-4947-95A2-55A086FD3E30}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="5" xr2:uid="{014C386D-7984-4947-95A2-55A086FD3E30}"/>
   </bookViews>
   <sheets>
     <sheet name="Not normalised" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="48">
   <si>
     <t>Fornavn</t>
   </si>
@@ -152,9 +152,6 @@
   </si>
   <si>
     <t>Status_id</t>
-  </si>
-  <si>
-    <t>På øager</t>
   </si>
   <si>
     <t>NULL</t>
@@ -347,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,6 +392,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -712,15 +713,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD8D0A4-6912-45A8-863D-BB1CFDA99329}">
   <dimension ref="B2:K6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.36328125" customWidth="1"/>
-    <col min="6" max="6" width="15.08984375" customWidth="1"/>
+    <col min="6" max="6" width="23.90625" customWidth="1"/>
     <col min="7" max="7" width="19.90625" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.35">
@@ -891,6 +895,7 @@
     <hyperlink ref="F6" r:id="rId4" xr:uid="{BFD834BA-D06F-4CFC-93B6-A5C0C4A09C01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -899,7 +904,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F5"/>
+      <selection activeCell="E1" sqref="E1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -995,6 +1000,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1003,7 +1009,7 @@
   <dimension ref="B2:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1059,8 +1065,8 @@
       <c r="G3" s="1">
         <v>1206</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
+      <c r="H3" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
@@ -1082,8 +1088,8 @@
       <c r="G4" s="1">
         <v>1229</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
+      <c r="H4" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
@@ -1105,8 +1111,8 @@
       <c r="G5" s="1">
         <v>2261</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>18</v>
+      <c r="H5" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
@@ -1128,8 +1134,8 @@
       <c r="G6" s="1">
         <v>1229</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>18</v>
+      <c r="H6" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1140,6 +1146,7 @@
     <hyperlink ref="E6" r:id="rId4" xr:uid="{6DBE4D0D-06DD-4630-A3A7-94468B366EBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1148,7 +1155,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1162,7 +1169,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1182,9 +1189,9 @@
         <v>33</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1207,7 +1214,7 @@
       <c r="G4" s="8">
         <v>1206</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1230,7 +1237,7 @@
       <c r="G5" s="8">
         <v>1229</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1253,7 +1260,7 @@
       <c r="G6" s="8">
         <v>2261</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1276,7 +1283,7 @@
       <c r="G7" s="8">
         <v>1229</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1288,6 +1295,7 @@
     <hyperlink ref="E7" r:id="rId4" xr:uid="{CF775D4C-7646-44ED-A3F1-447086D4265B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1296,7 +1304,7 @@
   <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B10" sqref="B10:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1406,6 +1414,9 @@
       <c r="E10" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="F10" s="20" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
@@ -1420,6 +1431,9 @@
       <c r="E11" s="1">
         <v>1206</v>
       </c>
+      <c r="F11" s="19" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
@@ -1434,6 +1448,9 @@
       <c r="E12" s="1">
         <v>1229</v>
       </c>
+      <c r="F12" s="19" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
@@ -1448,6 +1465,9 @@
       <c r="E13" s="1">
         <v>2261</v>
       </c>
+      <c r="F13" s="19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
@@ -1461,6 +1481,9 @@
       </c>
       <c r="E14" s="1">
         <v>1229</v>
+      </c>
+      <c r="F14" s="19" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1471,80 +1494,238 @@
     <hyperlink ref="F6" r:id="rId4" xr:uid="{A9BDB211-9BC5-4435-93EA-7078CE9F25AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22ADAFD-8341-4D49-B0BF-E777F9A9D5C1}">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="26.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>424255</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" s="3">
+        <v>424255</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="9">
+        <v>9816434</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>524252</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="3">
+        <v>524252</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="9">
+        <v>6524311</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>737363</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="3">
+        <v>737363</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="9">
+        <v>5252525</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>929282</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>36</v>
+      <c r="D6" s="3">
+        <v>929282</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="9">
+        <v>4424242</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1206</v>
+      </c>
+      <c r="H10" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1229</v>
+      </c>
+      <c r="H11" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2261</v>
+      </c>
+      <c r="H12" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1229</v>
+      </c>
+      <c r="H13" s="19" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{8474A4E1-EB2F-4708-8647-A24C73CE1E3F}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{EA65E8D4-D7D8-4A0D-9CDB-06AFEF2B2DDF}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{F5840080-6593-4F1F-B9A2-3525043DF59F}"/>
+    <hyperlink ref="H6" r:id="rId4" xr:uid="{A15F8247-8927-40F4-867C-2909C1CD7BAB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1552,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23DB2E8-57EF-4363-9089-900C172FE83F}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1566,7 +1747,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1580,10 +1761,10 @@
         <v>15</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1594,7 +1775,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="13">
         <v>2</v>
@@ -1608,7 +1789,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="13">
         <v>1</v>
@@ -1622,7 +1803,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="13">
         <v>0</v>
@@ -1636,15 +1817,15 @@
         <v>29</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1670,7 +1851,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
@@ -1678,7 +1859,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -1689,7 +1870,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1700,7 +1881,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -1711,14 +1892,15 @@
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1749,7 +1931,7 @@
         <v>35</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
@@ -1763,7 +1945,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
@@ -1801,5 +1983,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>